<commit_message>
Update Parts List - Trident 5 axis.xlsx
</commit_message>
<xml_diff>
--- a/Parts List - Trident 5 axis.xlsx
+++ b/Parts List - Trident 5 axis.xlsx
@@ -312,9 +312,6 @@
     <t>https://www.omgextrd.com/product-page/omgextrd-omg-dm1-extruder-upgrade</t>
   </si>
   <si>
-    <t>OMG V2S Extruder</t>
-  </si>
-  <si>
     <t>with M6 to M10 adapter and stepper motor</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>24V Fan 30x30x10mm</t>
+  </si>
+  <si>
+    <t>DM1 OMG V2S Extruder</t>
   </si>
 </sst>
 </file>
@@ -610,12 +610,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -928,12 +928,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="41.25" customHeight="1">
       <c r="A2" s="14" t="s">
@@ -1487,7 +1487,7 @@
       <c r="C50" s="23">
         <v>2</v>
       </c>
-      <c r="F50" s="33"/>
+      <c r="F50" s="32"/>
     </row>
     <row r="51" spans="1:6" ht="29.25" customHeight="1">
       <c r="A51" s="3" t="s">
@@ -1645,7 +1645,7 @@
       <c r="C65" s="23">
         <v>1</v>
       </c>
-      <c r="D65" s="34" t="s">
+      <c r="D65" s="33" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1673,27 +1673,27 @@
     </row>
     <row r="68" spans="1:5" ht="45.75" customHeight="1">
       <c r="A68" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B68" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="C68" s="23">
+        <v>1</v>
+      </c>
+      <c r="D68" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E68" s="33" t="s">
         <v>99</v>
-      </c>
-      <c r="C68" s="23">
-        <v>1</v>
-      </c>
-      <c r="D68" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E68" s="34" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="33.75" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C69" s="23">
         <v>1</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="70" spans="1:5" ht="33.75" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="23">
@@ -1710,7 +1710,7 @@
     </row>
     <row r="71" spans="1:5" ht="23.25" customHeight="1">
       <c r="A71" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="23">

</xml_diff>